<commit_message>
Update deployment Molpay SGD
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config Dev.xlsx
+++ b/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config Dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Molpaysgd\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC525F9-4ED0-4AC4-ACE1-F8CF8D43812D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01401163-93FA-42B4-A500-B27A640222BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="17268" windowHeight="8196" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -236,16 +236,16 @@
     <t>RPA044_MOLPAY_SG_MerchantID</t>
   </si>
   <si>
-    <t>RPA_Moon_GCaptcha_RuleId</t>
-  </si>
-  <si>
-    <t>RPA044_MOLPAY_Captcha_SiteKey</t>
-  </si>
-  <si>
     <t>TemplateMolpayFee</t>
   </si>
   <si>
     <t>C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\Template\Molpay Fee.xlsx</t>
+  </si>
+  <si>
+    <t>RPA044_MOLPAY_SG_Captcha_RuleId</t>
+  </si>
+  <si>
+    <t>RPA044_MOLPAY_SG_Captcha_SiteKey</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -721,10 +721,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2889,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2974,7 +2974,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -2982,7 +2982,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">

</xml_diff>

<commit_message>
Update Molpay new UI
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config Dev.xlsx
+++ b/Traveloka_DataAutomation_Portal_Molpaysgd/Data/Config Dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Molpaysgd\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01401163-93FA-42B4-A500-B27A640222BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F76A229-A1D8-464F-9796-1AF98889F37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1680" windowWidth="17268" windowHeight="8196" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -239,13 +239,13 @@
     <t>TemplateMolpayFee</t>
   </si>
   <si>
-    <t>C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgd\Data\Template\Molpay Fee.xlsx</t>
-  </si>
-  <si>
-    <t>RPA044_MOLPAY_SG_Captcha_RuleId</t>
-  </si>
-  <si>
     <t>RPA044_MOLPAY_SG_Captcha_SiteKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_CCaptcha_RuleId</t>
+  </si>
+  <si>
+    <t>Data\Template\Molpay Fee.xlsx</t>
   </si>
 </sst>
 </file>
@@ -326,9 +326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -366,7 +366,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -472,7 +472,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -614,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -724,7 +724,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2889,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2974,7 +2974,7 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">

</xml_diff>